<commit_message>
Tidy up the calibration spreadsheets.
</commit_message>
<xml_diff>
--- a/calibration/Tello Linear Rates.xlsx
+++ b/calibration/Tello Linear Rates.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stuart Golodetz\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\smglib\smg-rotory\calibration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAF63107-6DD3-4F82-B673-36F79A7F6DF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A4A7A90-18C8-4F92-AEE5-6A3DB6814398}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{867A7928-9A1E-4117-A2F9-3F4D8F336F48}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Chart1" sheetId="2" r:id="rId2"/>
-    <sheet name="Chart2" sheetId="3" r:id="rId3"/>
-    <sheet name="Chart3" sheetId="4" r:id="rId4"/>
+    <sheet name="Data" sheetId="1" r:id="rId1"/>
+    <sheet name="Forward Chart" sheetId="2" r:id="rId2"/>
+    <sheet name="Right Chart" sheetId="3" r:id="rId3"/>
+    <sheet name="Up Chart" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,33 +40,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="16">
   <si>
-    <t>Forward1</t>
-  </si>
-  <si>
-    <t>Forward2</t>
-  </si>
-  <si>
-    <t>Forward3</t>
-  </si>
-  <si>
-    <t>Right1</t>
-  </si>
-  <si>
-    <t>Right2</t>
-  </si>
-  <si>
-    <t>Right3</t>
-  </si>
-  <si>
-    <t>Up1</t>
-  </si>
-  <si>
-    <t>Up2</t>
-  </si>
-  <si>
-    <t>Up3</t>
-  </si>
-  <si>
     <t>Rate</t>
   </si>
   <si>
@@ -76,24 +49,59 @@
     <t>Variance</t>
   </si>
   <si>
-    <t>Forward Velocity</t>
+    <t>Forward1 (s)</t>
   </si>
   <si>
-    <t>Right Velocity</t>
+    <t>Forward2 (s)</t>
   </si>
   <si>
-    <t>Up Velocity</t>
+    <t>Forward3 (s)</t>
   </si>
   <si>
-    <t>Predicted</t>
+    <t>Right1 (s)</t>
+  </si>
+  <si>
+    <t>Right2 (s)</t>
+  </si>
+  <si>
+    <t>Right3 (s)</t>
+  </si>
+  <si>
+    <t>Up1 (s)</t>
+  </si>
+  <si>
+    <t>Up2 (s)</t>
+  </si>
+  <si>
+    <t>Up3 (s)</t>
+  </si>
+  <si>
+    <t>Forward Velocity (m/s)</t>
+  </si>
+  <si>
+    <t>Right Velocity (m/s)</t>
+  </si>
+  <si>
+    <t>Up Velocity (m/s)</t>
+  </si>
+  <si>
+    <t>Predicted (m/s)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -121,8 +129,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -154,37 +168,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
@@ -195,11 +179,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$10</c:f>
+              <c:f>Data!$B$10</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Forward Velocity</c:v>
+                  <c:v>Forward Velocity (m/s)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -278,7 +262,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$11:$A$17</c:f>
+              <c:f>Data!$A$11:$A$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -308,7 +292,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$11:$B$17</c:f>
+              <c:f>Data!$B$11:$B$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -361,6 +345,61 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Rate</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -423,6 +462,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Forward Velocity (m/s)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -512,37 +606,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
@@ -553,11 +617,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$F$10</c:f>
+              <c:f>Data!$F$10</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Right Velocity</c:v>
+                  <c:v>Right Velocity (m/s)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -650,7 +714,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$E$11:$E$17</c:f>
+              <c:f>Data!$E$11:$E$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -680,7 +744,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$F$11:$F$17</c:f>
+              <c:f>Data!$F$11:$F$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -733,6 +797,61 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Rate</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -795,6 +914,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Right Velocity (m/s)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -884,37 +1058,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
@@ -925,11 +1069,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$J$10</c:f>
+              <c:f>Data!$J$10</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Up Velocity</c:v>
+                  <c:v>Up Velocity (m/s)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1008,7 +1152,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$I$11:$I$17</c:f>
+              <c:f>Data!$I$11:$I$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -1038,7 +1182,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$J$11:$J$17</c:f>
+              <c:f>Data!$J$11:$J$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -1091,6 +1235,61 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Rate</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1153,6 +1352,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Up Velocity (m/s)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -2900,7 +3154,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{518E0B1E-D4EC-4E48-B828-61E42ACF3880}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="89" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="86" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -2911,7 +3165,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{3E2B9C7A-4E79-4279-B7FF-A2EAD5BF25C7}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="89" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="86" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -2922,7 +3176,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{B2458F31-019B-4C19-B71C-A1B211C9D7AF}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="89" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="86" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -2933,7 +3187,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9298112" cy="6070315"/>
+    <xdr:ext cx="8656674" cy="6282070"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -2966,7 +3220,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9298112" cy="6070315"/>
+    <xdr:ext cx="8656674" cy="6282070"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -2999,7 +3253,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9298112" cy="6070315"/>
+    <xdr:ext cx="8656674" cy="6282070"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -3331,846 +3585,850 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="12" bestFit="1" customWidth="1"/>
-    <col min="12" max="14" width="11" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="12" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.21875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.21875" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.21875" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="14" width="11" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="12" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="M1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="P1" s="1" t="s">
         <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G1" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1" t="s">
-        <v>4</v>
-      </c>
-      <c r="I1" t="s">
-        <v>5</v>
-      </c>
-      <c r="J1" t="s">
-        <v>10</v>
-      </c>
-      <c r="K1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L1" t="s">
-        <v>6</v>
-      </c>
-      <c r="M1" t="s">
-        <v>7</v>
-      </c>
-      <c r="N1" t="s">
-        <v>8</v>
-      </c>
-      <c r="O1" t="s">
-        <v>10</v>
-      </c>
-      <c r="P1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A2">
+      <c r="A2" s="2">
         <v>0.2</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="2">
         <v>14.985733400000001</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="2">
         <v>15.1502008999999</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="2">
         <v>13.2714739</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="2">
         <f>AVERAGE(B2:D2)</f>
         <v>14.469136066666636</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="2">
         <f>VARP(B2:D2)</f>
         <v>0.72170559249167709</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="2">
         <v>9.8298845999999998</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="2">
         <v>10.6401924999999</v>
       </c>
-      <c r="I2">
+      <c r="I2" s="2">
         <v>9.9630449999999993</v>
       </c>
-      <c r="J2">
+      <c r="J2" s="2">
         <f>AVERAGE(G2:I2)</f>
         <v>10.1443740333333</v>
       </c>
-      <c r="K2">
+      <c r="K2" s="2">
         <f>VARP(G2:I2)</f>
         <v>0.12587325796516932</v>
       </c>
-      <c r="L2">
+      <c r="L2" s="2">
         <v>23.4408092</v>
       </c>
-      <c r="M2">
+      <c r="M2" s="2">
         <v>23.869884099999901</v>
       </c>
-      <c r="N2">
+      <c r="N2" s="2">
         <v>24.662380200000001</v>
       </c>
-      <c r="O2">
+      <c r="O2" s="2">
         <f>AVERAGE(L2:N2)</f>
         <v>23.991024499999966</v>
       </c>
-      <c r="P2">
+      <c r="P2" s="2">
         <f>VARP(L2:N2)</f>
         <v>0.25604344959625508</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A3">
+      <c r="A3" s="2">
         <v>0.25</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="2">
         <v>10.4998174</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="2">
         <v>8.7638508999999996</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="2">
         <v>8.1363467000000007</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="2">
         <f t="shared" ref="E3:E8" si="0">AVERAGE(B3:D3)</f>
         <v>9.1333383333333327</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="2">
         <f t="shared" ref="F3:F8" si="1">VARP(B3:D3)</f>
         <v>0.99925943998870381</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="2">
         <v>7.6111675999999999</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="2">
         <v>7.3614913999999896</v>
       </c>
-      <c r="I3">
+      <c r="I3" s="2">
         <v>7.0392774999999999</v>
       </c>
-      <c r="J3">
+      <c r="J3" s="2">
         <f t="shared" ref="J3:J8" si="2">AVERAGE(G3:I3)</f>
         <v>7.3373121666666634</v>
       </c>
-      <c r="K3">
+      <c r="K3" s="2">
         <f t="shared" ref="K3:K8" si="3">VARP(G3:I3)</f>
         <v>5.4802032075295402E-2</v>
       </c>
-      <c r="L3">
+      <c r="L3" s="2">
         <v>17.000822700000001</v>
       </c>
-      <c r="M3">
+      <c r="M3" s="2">
         <v>15.665327899999999</v>
       </c>
-      <c r="N3">
+      <c r="N3" s="2">
         <v>15.7045391</v>
       </c>
-      <c r="O3">
+      <c r="O3" s="2">
         <f t="shared" ref="O3:O8" si="4">AVERAGE(L3:N3)</f>
         <v>16.123563233333332</v>
       </c>
-      <c r="P3">
+      <c r="P3" s="2">
         <f t="shared" ref="P3:P8" si="5">VARP(L3:N3)</f>
         <v>0.38504833896238272</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A4">
+      <c r="A4" s="2">
         <v>0.3</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="2">
         <v>7.7725942999999997</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="2">
         <v>7.7780339999999999</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="2">
         <v>7.9102442999999898</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="2">
         <f t="shared" si="0"/>
         <v>7.8202908666666628</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="2">
         <f t="shared" si="1"/>
         <v>4.0507418069082876E-3</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="2">
         <v>5.5894551000000003</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="2">
         <v>5.73077699999999</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="2">
         <v>5.9243838999999996</v>
       </c>
-      <c r="J4">
+      <c r="J4" s="2">
         <f t="shared" si="2"/>
         <v>5.7482053333333303</v>
       </c>
-      <c r="K4">
+      <c r="K4" s="2">
         <f t="shared" si="3"/>
         <v>1.8848090246295589E-2</v>
       </c>
-      <c r="L4">
+      <c r="L4" s="2">
         <v>12.247723499999999</v>
       </c>
-      <c r="M4">
+      <c r="M4" s="2">
         <v>12.522877299999999</v>
       </c>
-      <c r="N4">
+      <c r="N4" s="2">
         <v>11.8809325</v>
       </c>
-      <c r="O4">
+      <c r="O4" s="2">
         <f t="shared" si="4"/>
         <v>12.217177766666666</v>
       </c>
-      <c r="P4">
+      <c r="P4" s="2">
         <f t="shared" si="5"/>
         <v>6.9148708620275376E-2</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A5">
+      <c r="A5" s="2">
         <v>0.35</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="2">
         <v>7.1360035999999996</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="2">
         <v>6.7915549999999998</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="2">
         <v>7.7708576999999899</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="2">
         <f t="shared" si="0"/>
         <v>7.23280543333333</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="2">
         <f t="shared" si="1"/>
         <v>0.16452426050622534</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="2">
         <v>4.6389725999999998</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="2">
         <v>4.9879007</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="2">
         <v>5.0077641000000002</v>
       </c>
-      <c r="J5">
+      <c r="J5" s="2">
         <f t="shared" si="2"/>
         <v>4.8782124666666666</v>
       </c>
-      <c r="K5">
+      <c r="K5" s="2">
         <f t="shared" si="3"/>
         <v>2.8683616011268936E-2</v>
       </c>
-      <c r="L5">
+      <c r="L5" s="2">
         <v>10.1059482999999</v>
       </c>
-      <c r="M5">
+      <c r="M5" s="2">
         <v>9.3584156000000007</v>
       </c>
-      <c r="N5">
+      <c r="N5" s="2">
         <v>9.9681311000000008</v>
       </c>
-      <c r="O5">
+      <c r="O5" s="2">
         <f t="shared" si="4"/>
         <v>9.8108316666666351</v>
       </c>
-      <c r="P5">
+      <c r="P5" s="2">
         <f t="shared" si="5"/>
         <v>0.10550574545835578</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A6">
+      <c r="A6" s="2">
         <v>0.4</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="2">
         <v>4.6971752999999996</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="2">
         <v>5.4311432999999996</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="2">
         <v>5.4757270999999896</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="2">
         <f t="shared" si="0"/>
         <v>5.2013485666666632</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="2">
         <f t="shared" si="1"/>
         <v>0.12742662728107371</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="2">
         <v>3.9760548</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="2">
         <v>3.7294874</v>
       </c>
-      <c r="I6">
+      <c r="I6" s="2">
         <v>3.9137029000000001</v>
       </c>
-      <c r="J6">
+      <c r="J6" s="2">
         <f t="shared" si="2"/>
         <v>3.8730817000000002</v>
       </c>
-      <c r="K6">
+      <c r="K6" s="2">
         <f t="shared" si="3"/>
         <v>1.0957621401846668E-2</v>
       </c>
-      <c r="L6">
+      <c r="L6" s="2">
         <v>7.9951743000000004</v>
       </c>
-      <c r="M6">
+      <c r="M6" s="2">
         <v>8.1603966999999997</v>
       </c>
-      <c r="N6">
+      <c r="N6" s="2">
         <v>8.1105173999999902</v>
       </c>
-      <c r="O6">
+      <c r="O6" s="2">
         <f t="shared" si="4"/>
         <v>8.0886961333333307</v>
       </c>
-      <c r="P6">
+      <c r="P6" s="2">
         <f t="shared" si="5"/>
         <v>4.7878240830953748E-3</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A7">
+      <c r="A7" s="2">
         <v>0.45</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="2">
         <v>4.0834539000000003</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="2">
         <v>4.6342087000000003</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="2">
         <v>4.2684211999999899</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="2">
         <f t="shared" si="0"/>
         <v>4.3286945999999968</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="2">
         <f t="shared" si="1"/>
         <v>5.2371582994287076E-2</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="2">
         <v>3.0836100000000002</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="2">
         <v>3.24837989999999</v>
       </c>
-      <c r="I7">
+      <c r="I7" s="2">
         <v>3.1250353</v>
       </c>
-      <c r="J7">
+      <c r="J7" s="2">
         <f t="shared" si="2"/>
         <v>3.1523417333333299</v>
       </c>
-      <c r="K7">
+      <c r="K7" s="2">
         <f t="shared" si="3"/>
         <v>4.8976739750282404E-3</v>
       </c>
-      <c r="L7">
+      <c r="L7" s="2">
         <v>6.3538695999999897</v>
       </c>
-      <c r="M7">
+      <c r="M7" s="2">
         <v>6.44581789999999</v>
       </c>
-      <c r="N7">
+      <c r="N7" s="2">
         <v>6.7536078000000002</v>
       </c>
-      <c r="O7">
+      <c r="O7" s="2">
         <f t="shared" si="4"/>
         <v>6.5177650999999939</v>
       </c>
-      <c r="P7">
+      <c r="P7" s="2">
         <f t="shared" si="5"/>
         <v>2.9219971217128299E-2</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A8">
+      <c r="A8" s="2">
         <v>0.5</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="2">
         <v>3.2947538000000001</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="2">
         <v>3.5569136000000001</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="2">
         <v>3.5864981999999999</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="2">
         <f t="shared" si="0"/>
         <v>3.4793885333333332</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="2">
         <f t="shared" si="1"/>
         <v>1.7190867136062212E-2</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="2">
         <v>2.7345248999999998</v>
       </c>
-      <c r="H8">
+      <c r="H8" s="2">
         <v>2.7849328999999998</v>
       </c>
-      <c r="I8">
+      <c r="I8" s="2">
         <v>2.76675179999999</v>
       </c>
-      <c r="J8">
+      <c r="J8" s="2">
         <f t="shared" si="2"/>
         <v>2.7620698666666628</v>
       </c>
-      <c r="K8">
+      <c r="K8" s="2">
         <f t="shared" si="3"/>
         <v>4.3445466053552501E-4</v>
       </c>
-      <c r="L8">
+      <c r="L8" s="2">
         <v>5.6971260999999904</v>
       </c>
-      <c r="M8">
+      <c r="M8" s="2">
         <v>5.6282363999999898</v>
       </c>
-      <c r="N8">
+      <c r="N8" s="2">
         <v>5.5463661000000002</v>
       </c>
-      <c r="O8">
+      <c r="O8" s="2">
         <f t="shared" si="4"/>
         <v>5.6239095333333262</v>
       </c>
-      <c r="P8">
+      <c r="P8" s="2">
         <f t="shared" si="5"/>
         <v>3.7974571542417155E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
+    <row r="10" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E10" t="s">
-        <v>9</v>
-      </c>
-      <c r="F10" t="s">
+      <c r="E10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F10" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G10" t="s">
+      <c r="G10" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="I10" t="s">
-        <v>9</v>
-      </c>
-      <c r="J10" t="s">
+      <c r="I10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J10" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="K10" t="s">
+      <c r="K10" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A11">
+      <c r="A11" s="2">
         <v>0.2</v>
       </c>
-      <c r="B11">
-        <f>1/E2</f>
+      <c r="B11" s="2">
+        <f t="shared" ref="B11:B17" si="6">1/E2</f>
         <v>6.9112626724394166E-2</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="2">
         <f>0.6874*A11-0.0755</f>
         <v>6.1980000000000021E-2</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="2">
         <v>0.2</v>
       </c>
-      <c r="F11">
-        <f>1/J2</f>
+      <c r="F11" s="2">
+        <f t="shared" ref="F11:F17" si="7">1/J2</f>
         <v>9.8576806879765055E-2</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="2">
         <f>0.8832*E11-0.0875</f>
         <v>8.9140000000000025E-2</v>
       </c>
-      <c r="I11">
+      <c r="I11" s="2">
         <v>0.2</v>
       </c>
-      <c r="J11">
-        <f>1/O2</f>
+      <c r="J11" s="2">
+        <f t="shared" ref="J11:J17" si="8">1/O2</f>
         <v>4.1682254961642067E-2</v>
       </c>
-      <c r="K11">
+      <c r="K11" s="2">
         <f>0.4521*I11-0.0522</f>
         <v>3.8219999999999997E-2</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A12">
+      <c r="A12" s="2">
         <v>0.25</v>
       </c>
-      <c r="B12">
-        <f>1/E3</f>
+      <c r="B12" s="2">
+        <f t="shared" si="6"/>
         <v>0.10948899115566178</v>
       </c>
-      <c r="C12">
-        <f t="shared" ref="C12:C22" si="6">0.6874*A12-0.0755</f>
+      <c r="C12" s="2">
+        <f t="shared" ref="C12:C22" si="9">0.6874*A12-0.0755</f>
         <v>9.6350000000000005E-2</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="2">
         <v>0.25</v>
       </c>
-      <c r="F12">
-        <f>1/J3</f>
+      <c r="F12" s="2">
+        <f t="shared" si="7"/>
         <v>0.13628968991437901</v>
       </c>
-      <c r="G12">
-        <f t="shared" ref="G12:G22" si="7">0.8832*E12-0.0875</f>
+      <c r="G12" s="2">
+        <f t="shared" ref="G12:G22" si="10">0.8832*E12-0.0875</f>
         <v>0.1333</v>
       </c>
-      <c r="I12">
+      <c r="I12" s="2">
         <v>0.25</v>
       </c>
-      <c r="J12">
-        <f>1/O3</f>
+      <c r="J12" s="2">
+        <f t="shared" si="8"/>
         <v>6.2021030061930257E-2</v>
       </c>
-      <c r="K12">
-        <f t="shared" ref="K12:K22" si="8">0.4521*I12-0.0522</f>
+      <c r="K12" s="2">
+        <f t="shared" ref="K12:K22" si="11">0.4521*I12-0.0522</f>
         <v>6.0824999999999997E-2</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A13">
+      <c r="A13" s="2">
         <v>0.3</v>
       </c>
-      <c r="B13">
-        <f>1/E4</f>
+      <c r="B13" s="2">
+        <f t="shared" si="6"/>
         <v>0.12787248160582065</v>
       </c>
-      <c r="C13">
-        <f t="shared" si="6"/>
+      <c r="C13" s="2">
+        <f t="shared" si="9"/>
         <v>0.13072</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="2">
         <v>0.3</v>
       </c>
-      <c r="F13">
-        <f>1/J4</f>
+      <c r="F13" s="2">
+        <f t="shared" si="7"/>
         <v>0.1739673414589227</v>
       </c>
-      <c r="G13">
-        <f t="shared" si="7"/>
+      <c r="G13" s="2">
+        <f t="shared" si="10"/>
         <v>0.17745999999999998</v>
       </c>
-      <c r="I13">
+      <c r="I13" s="2">
         <v>0.3</v>
       </c>
-      <c r="J13">
-        <f>1/O4</f>
+      <c r="J13" s="2">
+        <f t="shared" si="8"/>
         <v>8.1851964430639523E-2</v>
       </c>
-      <c r="K13">
-        <f t="shared" si="8"/>
+      <c r="K13" s="2">
+        <f t="shared" si="11"/>
         <v>8.3430000000000004E-2</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A14">
+      <c r="A14" s="2">
         <v>0.35</v>
       </c>
-      <c r="B14">
-        <f>1/E5</f>
+      <c r="B14" s="2">
+        <f t="shared" si="6"/>
         <v>0.13825893828020994</v>
       </c>
-      <c r="C14">
-        <f t="shared" si="6"/>
+      <c r="C14" s="2">
+        <f t="shared" si="9"/>
         <v>0.16509000000000001</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="2">
         <v>0.35</v>
       </c>
-      <c r="F14">
-        <f>1/J5</f>
+      <c r="F14" s="2">
+        <f t="shared" si="7"/>
         <v>0.20499312131915207</v>
       </c>
-      <c r="G14">
-        <f t="shared" si="7"/>
+      <c r="G14" s="2">
+        <f t="shared" si="10"/>
         <v>0.22161999999999996</v>
       </c>
-      <c r="I14">
+      <c r="I14" s="2">
         <v>0.35</v>
       </c>
-      <c r="J14">
-        <f>1/O5</f>
+      <c r="J14" s="2">
+        <f t="shared" si="8"/>
         <v>0.10192815797641382</v>
       </c>
-      <c r="K14">
-        <f t="shared" si="8"/>
+      <c r="K14" s="2">
+        <f t="shared" si="11"/>
         <v>0.10603499999999999</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A15">
+      <c r="A15" s="2">
         <v>0.4</v>
       </c>
-      <c r="B15">
-        <f>1/E6</f>
+      <c r="B15" s="2">
+        <f t="shared" si="6"/>
         <v>0.19225783221078377</v>
       </c>
-      <c r="C15">
-        <f t="shared" si="6"/>
+      <c r="C15" s="2">
+        <f t="shared" si="9"/>
         <v>0.19946000000000003</v>
       </c>
-      <c r="E15">
+      <c r="E15" s="2">
         <v>0.4</v>
       </c>
-      <c r="F15">
-        <f>1/J6</f>
+      <c r="F15" s="2">
+        <f t="shared" si="7"/>
         <v>0.25819233299416328</v>
       </c>
-      <c r="G15">
-        <f t="shared" si="7"/>
+      <c r="G15" s="2">
+        <f t="shared" si="10"/>
         <v>0.26578000000000002</v>
       </c>
-      <c r="I15">
+      <c r="I15" s="2">
         <v>0.4</v>
       </c>
-      <c r="J15">
-        <f>1/O6</f>
+      <c r="J15" s="2">
+        <f t="shared" si="8"/>
         <v>0.12362931967230453</v>
       </c>
-      <c r="K15">
-        <f t="shared" si="8"/>
+      <c r="K15" s="2">
+        <f t="shared" si="11"/>
         <v>0.12864</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A16">
+      <c r="A16" s="2">
         <v>0.45</v>
       </c>
-      <c r="B16">
-        <f>1/E7</f>
+      <c r="B16" s="2">
+        <f t="shared" si="6"/>
         <v>0.2310165286319808</v>
       </c>
-      <c r="C16">
-        <f t="shared" si="6"/>
+      <c r="C16" s="2">
+        <f t="shared" si="9"/>
         <v>0.23382999999999998</v>
       </c>
-      <c r="E16">
+      <c r="E16" s="2">
         <v>0.45</v>
       </c>
-      <c r="F16">
-        <f>1/J7</f>
+      <c r="F16" s="2">
+        <f t="shared" si="7"/>
         <v>0.31722449042432532</v>
       </c>
-      <c r="G16">
-        <f t="shared" si="7"/>
+      <c r="G16" s="2">
+        <f t="shared" si="10"/>
         <v>0.30993999999999999</v>
       </c>
-      <c r="I16">
+      <c r="I16" s="2">
         <v>0.45</v>
       </c>
-      <c r="J16">
-        <f>1/O7</f>
+      <c r="J16" s="2">
+        <f t="shared" si="8"/>
         <v>0.15342682417321252</v>
       </c>
-      <c r="K16">
-        <f t="shared" si="8"/>
+      <c r="K16" s="2">
+        <f t="shared" si="11"/>
         <v>0.15124500000000002</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A17">
+      <c r="A17" s="2">
         <v>0.5</v>
       </c>
-      <c r="B17">
-        <f>1/E8</f>
+      <c r="B17" s="2">
+        <f t="shared" si="6"/>
         <v>0.2874068217503658</v>
       </c>
-      <c r="C17">
-        <f t="shared" si="6"/>
+      <c r="C17" s="2">
+        <f t="shared" si="9"/>
         <v>0.26819999999999999</v>
       </c>
-      <c r="E17">
+      <c r="E17" s="2">
         <v>0.5</v>
       </c>
-      <c r="F17">
-        <f>1/J8</f>
+      <c r="F17" s="2">
+        <f t="shared" si="7"/>
         <v>0.362047322577986</v>
       </c>
-      <c r="G17">
-        <f t="shared" si="7"/>
+      <c r="G17" s="2">
+        <f t="shared" si="10"/>
         <v>0.35409999999999997</v>
       </c>
-      <c r="I17">
+      <c r="I17" s="2">
         <v>0.5</v>
       </c>
-      <c r="J17">
-        <f>1/O8</f>
+      <c r="J17" s="2">
+        <f t="shared" si="8"/>
         <v>0.17781224859200281</v>
       </c>
-      <c r="K17">
-        <f t="shared" si="8"/>
+      <c r="K17" s="2">
+        <f t="shared" si="11"/>
         <v>0.17385</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A18">
+      <c r="A18" s="2">
         <v>0.6</v>
       </c>
-      <c r="C18">
-        <f t="shared" si="6"/>
+      <c r="C18" s="2">
+        <f t="shared" si="9"/>
         <v>0.33693999999999996</v>
       </c>
-      <c r="E18">
+      <c r="E18" s="2">
         <v>0.6</v>
       </c>
-      <c r="G18">
-        <f t="shared" si="7"/>
+      <c r="G18" s="2">
+        <f t="shared" si="10"/>
         <v>0.44241999999999992</v>
       </c>
-      <c r="I18">
+      <c r="I18" s="2">
         <v>0.6</v>
       </c>
-      <c r="K18">
-        <f t="shared" si="8"/>
+      <c r="K18" s="2">
+        <f t="shared" si="11"/>
         <v>0.21906</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A19">
+      <c r="A19" s="2">
         <v>0.7</v>
       </c>
-      <c r="C19">
-        <f t="shared" si="6"/>
+      <c r="C19" s="2">
+        <f t="shared" si="9"/>
         <v>0.40567999999999999</v>
       </c>
-      <c r="E19">
+      <c r="E19" s="2">
         <v>0.7</v>
       </c>
-      <c r="G19">
-        <f t="shared" si="7"/>
+      <c r="G19" s="2">
+        <f t="shared" si="10"/>
         <v>0.53073999999999988</v>
       </c>
-      <c r="I19">
+      <c r="I19" s="2">
         <v>0.7</v>
       </c>
-      <c r="K19">
-        <f t="shared" si="8"/>
+      <c r="K19" s="2">
+        <f t="shared" si="11"/>
         <v>0.26426999999999995</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A20">
+      <c r="A20" s="2">
         <v>0.8</v>
       </c>
-      <c r="C20">
-        <f t="shared" si="6"/>
+      <c r="C20" s="2">
+        <f t="shared" si="9"/>
         <v>0.47442000000000006</v>
       </c>
-      <c r="E20">
+      <c r="E20" s="2">
         <v>0.8</v>
       </c>
-      <c r="G20">
-        <f t="shared" si="7"/>
+      <c r="G20" s="2">
+        <f t="shared" si="10"/>
         <v>0.61906000000000005</v>
       </c>
-      <c r="I20">
+      <c r="I20" s="2">
         <v>0.8</v>
       </c>
-      <c r="K20">
-        <f t="shared" si="8"/>
+      <c r="K20" s="2">
+        <f t="shared" si="11"/>
         <v>0.30947999999999998</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A21">
+      <c r="A21" s="2">
         <v>0.9</v>
       </c>
-      <c r="C21">
-        <f t="shared" si="6"/>
+      <c r="C21" s="2">
+        <f t="shared" si="9"/>
         <v>0.54315999999999998</v>
       </c>
-      <c r="E21">
+      <c r="E21" s="2">
         <v>0.9</v>
       </c>
-      <c r="G21">
-        <f t="shared" si="7"/>
+      <c r="G21" s="2">
+        <f t="shared" si="10"/>
         <v>0.70738000000000001</v>
       </c>
-      <c r="I21">
+      <c r="I21" s="2">
         <v>0.9</v>
       </c>
-      <c r="K21">
-        <f t="shared" si="8"/>
+      <c r="K21" s="2">
+        <f t="shared" si="11"/>
         <v>0.35469000000000001</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A22">
+      <c r="A22" s="2">
         <v>1</v>
       </c>
-      <c r="C22">
-        <f t="shared" si="6"/>
+      <c r="C22" s="2">
+        <f t="shared" si="9"/>
         <v>0.6119</v>
       </c>
-      <c r="E22">
+      <c r="E22" s="2">
         <v>1</v>
       </c>
-      <c r="G22">
-        <f t="shared" si="7"/>
+      <c r="G22" s="2">
+        <f t="shared" si="10"/>
         <v>0.79569999999999996</v>
       </c>
-      <c r="I22">
+      <c r="I22" s="2">
         <v>1</v>
       </c>
-      <c r="K22">
-        <f t="shared" si="8"/>
+      <c r="K22" s="2">
+        <f t="shared" si="11"/>
         <v>0.39989999999999998</v>
       </c>
     </row>

</xml_diff>